<commit_message>
feat: update to version 9.14
</commit_message>
<xml_diff>
--- a/site/StructureDefinition-appointment-mode.xlsx
+++ b/site/StructureDefinition-appointment-mode.xlsx
@@ -30,7 +30,7 @@
     <t>Version</t>
   </si>
   <si>
-    <t>0.9.11</t>
+    <t>0.9.15</t>
   </si>
   <si>
     <t>Name</t>
@@ -57,7 +57,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2025-09-10T15:54:27-03:00</t>
+    <t>2025-10-03T11:11:24-03:00</t>
   </si>
   <si>
     <t>Publisher</t>

</xml_diff>

<commit_message>
feat: update to version 9.14 (#4)
</commit_message>
<xml_diff>
--- a/site/StructureDefinition-appointment-mode.xlsx
+++ b/site/StructureDefinition-appointment-mode.xlsx
@@ -30,7 +30,7 @@
     <t>Version</t>
   </si>
   <si>
-    <t>0.9.11</t>
+    <t>0.9.15</t>
   </si>
   <si>
     <t>Name</t>
@@ -57,7 +57,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2025-09-10T15:54:27-03:00</t>
+    <t>2025-10-03T11:11:24-03:00</t>
   </si>
   <si>
     <t>Publisher</t>

</xml_diff>

<commit_message>
feat: update to 0.9.20
</commit_message>
<xml_diff>
--- a/site/StructureDefinition-appointment-mode.xlsx
+++ b/site/StructureDefinition-appointment-mode.xlsx
@@ -30,7 +30,7 @@
     <t>Version</t>
   </si>
   <si>
-    <t>0.9.15</t>
+    <t>0.9.20</t>
   </si>
   <si>
     <t>Name</t>
@@ -57,7 +57,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2025-10-30T18:43:23-03:00</t>
+    <t>2025-11-18T19:57:13-03:00</t>
   </si>
   <si>
     <t>Publisher</t>

</xml_diff>

<commit_message>
feat: update to 0.9.20 (#6)
</commit_message>
<xml_diff>
--- a/site/StructureDefinition-appointment-mode.xlsx
+++ b/site/StructureDefinition-appointment-mode.xlsx
@@ -30,7 +30,7 @@
     <t>Version</t>
   </si>
   <si>
-    <t>0.9.15</t>
+    <t>0.9.20</t>
   </si>
   <si>
     <t>Name</t>
@@ -57,7 +57,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2025-10-30T18:43:23-03:00</t>
+    <t>2025-11-18T19:57:13-03:00</t>
   </si>
   <si>
     <t>Publisher</t>

</xml_diff>

<commit_message>
feat: update to 0.9.21
</commit_message>
<xml_diff>
--- a/site/StructureDefinition-appointment-mode.xlsx
+++ b/site/StructureDefinition-appointment-mode.xlsx
@@ -30,7 +30,7 @@
     <t>Version</t>
   </si>
   <si>
-    <t>0.9.20</t>
+    <t>0.9.21</t>
   </si>
   <si>
     <t>Name</t>
@@ -57,7 +57,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2025-11-18T19:57:13-03:00</t>
+    <t>2025-11-24T17:38:48-05:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -663,42 +663,42 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" width="16.80078125" customWidth="true" bestFit="true"/>
-    <col min="2" max="2" width="16.80078125" customWidth="true" bestFit="true"/>
-    <col min="3" max="3" width="10.8515625" customWidth="true" bestFit="true" hidden="true"/>
-    <col min="4" max="4" width="7.6796875" customWidth="true" bestFit="true" hidden="true"/>
-    <col min="5" max="5" width="5.80859375" customWidth="true" bestFit="true"/>
-    <col min="6" max="6" width="4.23828125" customWidth="true" bestFit="true"/>
-    <col min="7" max="7" width="4.65625" customWidth="true" bestFit="true"/>
-    <col min="8" max="8" width="13.953125" customWidth="true" bestFit="true"/>
-    <col min="9" max="9" width="11.3671875" customWidth="true" bestFit="true"/>
+    <col min="1" max="1" width="16.41796875" customWidth="true" bestFit="true"/>
+    <col min="2" max="2" width="16.41796875" customWidth="true" bestFit="true"/>
+    <col min="3" max="3" width="9.79296875" customWidth="true" bestFit="true" hidden="true"/>
+    <col min="4" max="4" width="7.046875" customWidth="true" bestFit="true" hidden="true"/>
+    <col min="5" max="5" width="5.30078125" customWidth="true" bestFit="true"/>
+    <col min="6" max="6" width="3.953125" customWidth="true" bestFit="true"/>
+    <col min="7" max="7" width="4.265625" customWidth="true" bestFit="true"/>
+    <col min="8" max="8" width="12.6875" customWidth="true" bestFit="true"/>
+    <col min="9" max="9" width="10.51171875" customWidth="true" bestFit="true"/>
     <col min="10" max="10" width="20.703125" customWidth="true" bestFit="true"/>
-    <col min="11" max="11" width="8.609375" customWidth="true" bestFit="true"/>
+    <col min="11" max="11" width="8.3984375" customWidth="true" bestFit="true"/>
     <col min="12" max="12" width="100.703125" customWidth="true" bestFit="true"/>
     <col min="13" max="13" width="100.703125" customWidth="true" bestFit="true"/>
     <col min="14" max="14" width="100.703125" customWidth="true" bestFit="true"/>
-    <col min="15" max="15" width="13.4296875" customWidth="true" bestFit="true"/>
+    <col min="15" max="15" width="12.26171875" customWidth="true" bestFit="true"/>
     <col min="16" max="16" width="20.703125" customWidth="true" bestFit="true"/>
     <col min="17" max="17" width="20.703125" customWidth="true" bestFit="true"/>
     <col min="18" max="18" width="20.703125" customWidth="true" bestFit="true"/>
     <col min="19" max="19" width="20.703125" customWidth="true" bestFit="true"/>
     <col min="20" max="20" width="8.53515625" customWidth="true" bestFit="true"/>
-    <col min="21" max="21" width="14.72265625" customWidth="true" bestFit="true"/>
-    <col min="22" max="22" width="15.13671875" customWidth="true" bestFit="true"/>
-    <col min="23" max="23" width="16.3203125" customWidth="true" bestFit="true"/>
-    <col min="24" max="24" width="16.16796875" customWidth="true" bestFit="true"/>
-    <col min="25" max="25" width="18.49609375" customWidth="true" bestFit="true"/>
-    <col min="26" max="26" width="16.828125" customWidth="true" bestFit="true"/>
-    <col min="27" max="27" width="5.44140625" customWidth="true" bestFit="true"/>
-    <col min="28" max="28" width="19.4765625" customWidth="true" bestFit="true"/>
-    <col min="29" max="29" width="36.0390625" customWidth="true" bestFit="true"/>
-    <col min="30" max="30" width="14.7578125" customWidth="true" bestFit="true"/>
-    <col min="31" max="31" width="12.359375" customWidth="true" bestFit="true" hidden="true"/>
-    <col min="32" max="32" width="15.59375" customWidth="true" bestFit="true" hidden="true"/>
-    <col min="33" max="33" width="9.046875" customWidth="true" bestFit="true" hidden="true"/>
-    <col min="34" max="34" width="9.46484375" customWidth="true" bestFit="true"/>
+    <col min="21" max="21" width="13.609375" customWidth="true" bestFit="true"/>
+    <col min="22" max="22" width="13.91796875" customWidth="true" bestFit="true"/>
+    <col min="23" max="23" width="15.01171875" customWidth="true" bestFit="true"/>
+    <col min="24" max="24" width="14.62890625" customWidth="true" bestFit="true"/>
+    <col min="25" max="25" width="17.08203125" customWidth="true" bestFit="true"/>
+    <col min="26" max="26" width="15.18359375" customWidth="true" bestFit="true"/>
+    <col min="27" max="27" width="5.07421875" customWidth="true" bestFit="true"/>
+    <col min="28" max="28" width="17.98046875" customWidth="true" bestFit="true"/>
+    <col min="29" max="29" width="34.578125" customWidth="true" bestFit="true"/>
+    <col min="30" max="30" width="13.54296875" customWidth="true" bestFit="true"/>
+    <col min="31" max="31" width="11.3203125" customWidth="true" bestFit="true" hidden="true"/>
+    <col min="32" max="32" width="15.046875" customWidth="true" bestFit="true" hidden="true"/>
+    <col min="33" max="33" width="8.22265625" customWidth="true" bestFit="true" hidden="true"/>
+    <col min="34" max="34" width="8.53125" customWidth="true" bestFit="true"/>
     <col min="35" max="35" width="100.703125" customWidth="true"/>
-    <col min="37" max="37" width="21.4140625" customWidth="true" bestFit="true"/>
+    <col min="37" max="37" width="19.5625" customWidth="true" bestFit="true"/>
   </cols>
   <sheetData>
     <row r="1">

</xml_diff>

<commit_message>
feat: update to 0.9.21 (#7)
</commit_message>
<xml_diff>
--- a/site/StructureDefinition-appointment-mode.xlsx
+++ b/site/StructureDefinition-appointment-mode.xlsx
@@ -30,7 +30,7 @@
     <t>Version</t>
   </si>
   <si>
-    <t>0.9.20</t>
+    <t>0.9.21</t>
   </si>
   <si>
     <t>Name</t>
@@ -57,7 +57,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2025-11-18T19:57:13-03:00</t>
+    <t>2025-11-24T17:38:48-05:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -663,42 +663,42 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" width="16.80078125" customWidth="true" bestFit="true"/>
-    <col min="2" max="2" width="16.80078125" customWidth="true" bestFit="true"/>
-    <col min="3" max="3" width="10.8515625" customWidth="true" bestFit="true" hidden="true"/>
-    <col min="4" max="4" width="7.6796875" customWidth="true" bestFit="true" hidden="true"/>
-    <col min="5" max="5" width="5.80859375" customWidth="true" bestFit="true"/>
-    <col min="6" max="6" width="4.23828125" customWidth="true" bestFit="true"/>
-    <col min="7" max="7" width="4.65625" customWidth="true" bestFit="true"/>
-    <col min="8" max="8" width="13.953125" customWidth="true" bestFit="true"/>
-    <col min="9" max="9" width="11.3671875" customWidth="true" bestFit="true"/>
+    <col min="1" max="1" width="16.41796875" customWidth="true" bestFit="true"/>
+    <col min="2" max="2" width="16.41796875" customWidth="true" bestFit="true"/>
+    <col min="3" max="3" width="9.79296875" customWidth="true" bestFit="true" hidden="true"/>
+    <col min="4" max="4" width="7.046875" customWidth="true" bestFit="true" hidden="true"/>
+    <col min="5" max="5" width="5.30078125" customWidth="true" bestFit="true"/>
+    <col min="6" max="6" width="3.953125" customWidth="true" bestFit="true"/>
+    <col min="7" max="7" width="4.265625" customWidth="true" bestFit="true"/>
+    <col min="8" max="8" width="12.6875" customWidth="true" bestFit="true"/>
+    <col min="9" max="9" width="10.51171875" customWidth="true" bestFit="true"/>
     <col min="10" max="10" width="20.703125" customWidth="true" bestFit="true"/>
-    <col min="11" max="11" width="8.609375" customWidth="true" bestFit="true"/>
+    <col min="11" max="11" width="8.3984375" customWidth="true" bestFit="true"/>
     <col min="12" max="12" width="100.703125" customWidth="true" bestFit="true"/>
     <col min="13" max="13" width="100.703125" customWidth="true" bestFit="true"/>
     <col min="14" max="14" width="100.703125" customWidth="true" bestFit="true"/>
-    <col min="15" max="15" width="13.4296875" customWidth="true" bestFit="true"/>
+    <col min="15" max="15" width="12.26171875" customWidth="true" bestFit="true"/>
     <col min="16" max="16" width="20.703125" customWidth="true" bestFit="true"/>
     <col min="17" max="17" width="20.703125" customWidth="true" bestFit="true"/>
     <col min="18" max="18" width="20.703125" customWidth="true" bestFit="true"/>
     <col min="19" max="19" width="20.703125" customWidth="true" bestFit="true"/>
     <col min="20" max="20" width="8.53515625" customWidth="true" bestFit="true"/>
-    <col min="21" max="21" width="14.72265625" customWidth="true" bestFit="true"/>
-    <col min="22" max="22" width="15.13671875" customWidth="true" bestFit="true"/>
-    <col min="23" max="23" width="16.3203125" customWidth="true" bestFit="true"/>
-    <col min="24" max="24" width="16.16796875" customWidth="true" bestFit="true"/>
-    <col min="25" max="25" width="18.49609375" customWidth="true" bestFit="true"/>
-    <col min="26" max="26" width="16.828125" customWidth="true" bestFit="true"/>
-    <col min="27" max="27" width="5.44140625" customWidth="true" bestFit="true"/>
-    <col min="28" max="28" width="19.4765625" customWidth="true" bestFit="true"/>
-    <col min="29" max="29" width="36.0390625" customWidth="true" bestFit="true"/>
-    <col min="30" max="30" width="14.7578125" customWidth="true" bestFit="true"/>
-    <col min="31" max="31" width="12.359375" customWidth="true" bestFit="true" hidden="true"/>
-    <col min="32" max="32" width="15.59375" customWidth="true" bestFit="true" hidden="true"/>
-    <col min="33" max="33" width="9.046875" customWidth="true" bestFit="true" hidden="true"/>
-    <col min="34" max="34" width="9.46484375" customWidth="true" bestFit="true"/>
+    <col min="21" max="21" width="13.609375" customWidth="true" bestFit="true"/>
+    <col min="22" max="22" width="13.91796875" customWidth="true" bestFit="true"/>
+    <col min="23" max="23" width="15.01171875" customWidth="true" bestFit="true"/>
+    <col min="24" max="24" width="14.62890625" customWidth="true" bestFit="true"/>
+    <col min="25" max="25" width="17.08203125" customWidth="true" bestFit="true"/>
+    <col min="26" max="26" width="15.18359375" customWidth="true" bestFit="true"/>
+    <col min="27" max="27" width="5.07421875" customWidth="true" bestFit="true"/>
+    <col min="28" max="28" width="17.98046875" customWidth="true" bestFit="true"/>
+    <col min="29" max="29" width="34.578125" customWidth="true" bestFit="true"/>
+    <col min="30" max="30" width="13.54296875" customWidth="true" bestFit="true"/>
+    <col min="31" max="31" width="11.3203125" customWidth="true" bestFit="true" hidden="true"/>
+    <col min="32" max="32" width="15.046875" customWidth="true" bestFit="true" hidden="true"/>
+    <col min="33" max="33" width="8.22265625" customWidth="true" bestFit="true" hidden="true"/>
+    <col min="34" max="34" width="8.53125" customWidth="true" bestFit="true"/>
     <col min="35" max="35" width="100.703125" customWidth="true"/>
-    <col min="37" max="37" width="21.4140625" customWidth="true" bestFit="true"/>
+    <col min="37" max="37" width="19.5625" customWidth="true" bestFit="true"/>
   </cols>
   <sheetData>
     <row r="1">

</xml_diff>

<commit_message>
feat: bump to 0.9.23
</commit_message>
<xml_diff>
--- a/site/StructureDefinition-appointment-mode.xlsx
+++ b/site/StructureDefinition-appointment-mode.xlsx
@@ -30,7 +30,7 @@
     <t>Version</t>
   </si>
   <si>
-    <t>0.9.22</t>
+    <t>0.9.23</t>
   </si>
   <si>
     <t>Name</t>
@@ -57,7 +57,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2025-11-25T17:07:48-05:00</t>
+    <t>2025-12-02T11:10:54-03:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -663,42 +663,42 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" width="16.41796875" customWidth="true" bestFit="true"/>
-    <col min="2" max="2" width="16.41796875" customWidth="true" bestFit="true"/>
-    <col min="3" max="3" width="9.79296875" customWidth="true" bestFit="true" hidden="true"/>
-    <col min="4" max="4" width="7.046875" customWidth="true" bestFit="true" hidden="true"/>
-    <col min="5" max="5" width="5.30078125" customWidth="true" bestFit="true"/>
-    <col min="6" max="6" width="3.953125" customWidth="true" bestFit="true"/>
-    <col min="7" max="7" width="4.265625" customWidth="true" bestFit="true"/>
-    <col min="8" max="8" width="12.6875" customWidth="true" bestFit="true"/>
-    <col min="9" max="9" width="10.51171875" customWidth="true" bestFit="true"/>
+    <col min="1" max="1" width="16.80078125" customWidth="true" bestFit="true"/>
+    <col min="2" max="2" width="16.80078125" customWidth="true" bestFit="true"/>
+    <col min="3" max="3" width="10.8515625" customWidth="true" bestFit="true" hidden="true"/>
+    <col min="4" max="4" width="7.6796875" customWidth="true" bestFit="true" hidden="true"/>
+    <col min="5" max="5" width="5.80859375" customWidth="true" bestFit="true"/>
+    <col min="6" max="6" width="4.23828125" customWidth="true" bestFit="true"/>
+    <col min="7" max="7" width="4.65625" customWidth="true" bestFit="true"/>
+    <col min="8" max="8" width="13.953125" customWidth="true" bestFit="true"/>
+    <col min="9" max="9" width="11.3671875" customWidth="true" bestFit="true"/>
     <col min="10" max="10" width="20.703125" customWidth="true" bestFit="true"/>
-    <col min="11" max="11" width="8.3984375" customWidth="true" bestFit="true"/>
+    <col min="11" max="11" width="8.609375" customWidth="true" bestFit="true"/>
     <col min="12" max="12" width="100.703125" customWidth="true" bestFit="true"/>
     <col min="13" max="13" width="100.703125" customWidth="true" bestFit="true"/>
     <col min="14" max="14" width="100.703125" customWidth="true" bestFit="true"/>
-    <col min="15" max="15" width="12.26171875" customWidth="true" bestFit="true"/>
+    <col min="15" max="15" width="13.4296875" customWidth="true" bestFit="true"/>
     <col min="16" max="16" width="20.703125" customWidth="true" bestFit="true"/>
     <col min="17" max="17" width="20.703125" customWidth="true" bestFit="true"/>
     <col min="18" max="18" width="20.703125" customWidth="true" bestFit="true"/>
     <col min="19" max="19" width="20.703125" customWidth="true" bestFit="true"/>
     <col min="20" max="20" width="8.53515625" customWidth="true" bestFit="true"/>
-    <col min="21" max="21" width="13.609375" customWidth="true" bestFit="true"/>
-    <col min="22" max="22" width="13.91796875" customWidth="true" bestFit="true"/>
-    <col min="23" max="23" width="15.01171875" customWidth="true" bestFit="true"/>
-    <col min="24" max="24" width="14.62890625" customWidth="true" bestFit="true"/>
-    <col min="25" max="25" width="17.08203125" customWidth="true" bestFit="true"/>
-    <col min="26" max="26" width="15.18359375" customWidth="true" bestFit="true"/>
-    <col min="27" max="27" width="5.07421875" customWidth="true" bestFit="true"/>
-    <col min="28" max="28" width="17.98046875" customWidth="true" bestFit="true"/>
-    <col min="29" max="29" width="34.578125" customWidth="true" bestFit="true"/>
-    <col min="30" max="30" width="13.54296875" customWidth="true" bestFit="true"/>
-    <col min="31" max="31" width="11.3203125" customWidth="true" bestFit="true" hidden="true"/>
-    <col min="32" max="32" width="15.046875" customWidth="true" bestFit="true" hidden="true"/>
-    <col min="33" max="33" width="8.22265625" customWidth="true" bestFit="true" hidden="true"/>
-    <col min="34" max="34" width="8.53125" customWidth="true" bestFit="true"/>
+    <col min="21" max="21" width="14.72265625" customWidth="true" bestFit="true"/>
+    <col min="22" max="22" width="15.13671875" customWidth="true" bestFit="true"/>
+    <col min="23" max="23" width="16.3203125" customWidth="true" bestFit="true"/>
+    <col min="24" max="24" width="16.16796875" customWidth="true" bestFit="true"/>
+    <col min="25" max="25" width="18.49609375" customWidth="true" bestFit="true"/>
+    <col min="26" max="26" width="16.828125" customWidth="true" bestFit="true"/>
+    <col min="27" max="27" width="5.44140625" customWidth="true" bestFit="true"/>
+    <col min="28" max="28" width="19.4765625" customWidth="true" bestFit="true"/>
+    <col min="29" max="29" width="36.0390625" customWidth="true" bestFit="true"/>
+    <col min="30" max="30" width="14.7578125" customWidth="true" bestFit="true"/>
+    <col min="31" max="31" width="12.359375" customWidth="true" bestFit="true" hidden="true"/>
+    <col min="32" max="32" width="15.59375" customWidth="true" bestFit="true" hidden="true"/>
+    <col min="33" max="33" width="9.046875" customWidth="true" bestFit="true" hidden="true"/>
+    <col min="34" max="34" width="9.46484375" customWidth="true" bestFit="true"/>
     <col min="35" max="35" width="100.703125" customWidth="true"/>
-    <col min="37" max="37" width="19.5625" customWidth="true" bestFit="true"/>
+    <col min="37" max="37" width="21.4140625" customWidth="true" bestFit="true"/>
   </cols>
   <sheetData>
     <row r="1">

</xml_diff>

<commit_message>
feat: bump to 0.9.23 (#10)
</commit_message>
<xml_diff>
--- a/site/StructureDefinition-appointment-mode.xlsx
+++ b/site/StructureDefinition-appointment-mode.xlsx
@@ -30,7 +30,7 @@
     <t>Version</t>
   </si>
   <si>
-    <t>0.9.22</t>
+    <t>0.9.23</t>
   </si>
   <si>
     <t>Name</t>
@@ -57,7 +57,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2025-11-25T17:07:48-05:00</t>
+    <t>2025-12-02T11:10:54-03:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -663,42 +663,42 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" width="16.41796875" customWidth="true" bestFit="true"/>
-    <col min="2" max="2" width="16.41796875" customWidth="true" bestFit="true"/>
-    <col min="3" max="3" width="9.79296875" customWidth="true" bestFit="true" hidden="true"/>
-    <col min="4" max="4" width="7.046875" customWidth="true" bestFit="true" hidden="true"/>
-    <col min="5" max="5" width="5.30078125" customWidth="true" bestFit="true"/>
-    <col min="6" max="6" width="3.953125" customWidth="true" bestFit="true"/>
-    <col min="7" max="7" width="4.265625" customWidth="true" bestFit="true"/>
-    <col min="8" max="8" width="12.6875" customWidth="true" bestFit="true"/>
-    <col min="9" max="9" width="10.51171875" customWidth="true" bestFit="true"/>
+    <col min="1" max="1" width="16.80078125" customWidth="true" bestFit="true"/>
+    <col min="2" max="2" width="16.80078125" customWidth="true" bestFit="true"/>
+    <col min="3" max="3" width="10.8515625" customWidth="true" bestFit="true" hidden="true"/>
+    <col min="4" max="4" width="7.6796875" customWidth="true" bestFit="true" hidden="true"/>
+    <col min="5" max="5" width="5.80859375" customWidth="true" bestFit="true"/>
+    <col min="6" max="6" width="4.23828125" customWidth="true" bestFit="true"/>
+    <col min="7" max="7" width="4.65625" customWidth="true" bestFit="true"/>
+    <col min="8" max="8" width="13.953125" customWidth="true" bestFit="true"/>
+    <col min="9" max="9" width="11.3671875" customWidth="true" bestFit="true"/>
     <col min="10" max="10" width="20.703125" customWidth="true" bestFit="true"/>
-    <col min="11" max="11" width="8.3984375" customWidth="true" bestFit="true"/>
+    <col min="11" max="11" width="8.609375" customWidth="true" bestFit="true"/>
     <col min="12" max="12" width="100.703125" customWidth="true" bestFit="true"/>
     <col min="13" max="13" width="100.703125" customWidth="true" bestFit="true"/>
     <col min="14" max="14" width="100.703125" customWidth="true" bestFit="true"/>
-    <col min="15" max="15" width="12.26171875" customWidth="true" bestFit="true"/>
+    <col min="15" max="15" width="13.4296875" customWidth="true" bestFit="true"/>
     <col min="16" max="16" width="20.703125" customWidth="true" bestFit="true"/>
     <col min="17" max="17" width="20.703125" customWidth="true" bestFit="true"/>
     <col min="18" max="18" width="20.703125" customWidth="true" bestFit="true"/>
     <col min="19" max="19" width="20.703125" customWidth="true" bestFit="true"/>
     <col min="20" max="20" width="8.53515625" customWidth="true" bestFit="true"/>
-    <col min="21" max="21" width="13.609375" customWidth="true" bestFit="true"/>
-    <col min="22" max="22" width="13.91796875" customWidth="true" bestFit="true"/>
-    <col min="23" max="23" width="15.01171875" customWidth="true" bestFit="true"/>
-    <col min="24" max="24" width="14.62890625" customWidth="true" bestFit="true"/>
-    <col min="25" max="25" width="17.08203125" customWidth="true" bestFit="true"/>
-    <col min="26" max="26" width="15.18359375" customWidth="true" bestFit="true"/>
-    <col min="27" max="27" width="5.07421875" customWidth="true" bestFit="true"/>
-    <col min="28" max="28" width="17.98046875" customWidth="true" bestFit="true"/>
-    <col min="29" max="29" width="34.578125" customWidth="true" bestFit="true"/>
-    <col min="30" max="30" width="13.54296875" customWidth="true" bestFit="true"/>
-    <col min="31" max="31" width="11.3203125" customWidth="true" bestFit="true" hidden="true"/>
-    <col min="32" max="32" width="15.046875" customWidth="true" bestFit="true" hidden="true"/>
-    <col min="33" max="33" width="8.22265625" customWidth="true" bestFit="true" hidden="true"/>
-    <col min="34" max="34" width="8.53125" customWidth="true" bestFit="true"/>
+    <col min="21" max="21" width="14.72265625" customWidth="true" bestFit="true"/>
+    <col min="22" max="22" width="15.13671875" customWidth="true" bestFit="true"/>
+    <col min="23" max="23" width="16.3203125" customWidth="true" bestFit="true"/>
+    <col min="24" max="24" width="16.16796875" customWidth="true" bestFit="true"/>
+    <col min="25" max="25" width="18.49609375" customWidth="true" bestFit="true"/>
+    <col min="26" max="26" width="16.828125" customWidth="true" bestFit="true"/>
+    <col min="27" max="27" width="5.44140625" customWidth="true" bestFit="true"/>
+    <col min="28" max="28" width="19.4765625" customWidth="true" bestFit="true"/>
+    <col min="29" max="29" width="36.0390625" customWidth="true" bestFit="true"/>
+    <col min="30" max="30" width="14.7578125" customWidth="true" bestFit="true"/>
+    <col min="31" max="31" width="12.359375" customWidth="true" bestFit="true" hidden="true"/>
+    <col min="32" max="32" width="15.59375" customWidth="true" bestFit="true" hidden="true"/>
+    <col min="33" max="33" width="9.046875" customWidth="true" bestFit="true" hidden="true"/>
+    <col min="34" max="34" width="9.46484375" customWidth="true" bestFit="true"/>
     <col min="35" max="35" width="100.703125" customWidth="true"/>
-    <col min="37" max="37" width="19.5625" customWidth="true" bestFit="true"/>
+    <col min="37" max="37" width="21.4140625" customWidth="true" bestFit="true"/>
   </cols>
   <sheetData>
     <row r="1">

</xml_diff>

<commit_message>
feat: bump to 0.9.24
</commit_message>
<xml_diff>
--- a/site/StructureDefinition-appointment-mode.xlsx
+++ b/site/StructureDefinition-appointment-mode.xlsx
@@ -30,7 +30,7 @@
     <t>Version</t>
   </si>
   <si>
-    <t>0.9.23</t>
+    <t>0.9.24</t>
   </si>
   <si>
     <t>Name</t>
@@ -57,7 +57,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2025-12-02T11:10:54-03:00</t>
+    <t>2025-12-08T15:17:38-05:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -663,42 +663,42 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" width="16.80078125" customWidth="true" bestFit="true"/>
-    <col min="2" max="2" width="16.80078125" customWidth="true" bestFit="true"/>
-    <col min="3" max="3" width="10.8515625" customWidth="true" bestFit="true" hidden="true"/>
-    <col min="4" max="4" width="7.6796875" customWidth="true" bestFit="true" hidden="true"/>
-    <col min="5" max="5" width="5.80859375" customWidth="true" bestFit="true"/>
-    <col min="6" max="6" width="4.23828125" customWidth="true" bestFit="true"/>
-    <col min="7" max="7" width="4.65625" customWidth="true" bestFit="true"/>
-    <col min="8" max="8" width="13.953125" customWidth="true" bestFit="true"/>
-    <col min="9" max="9" width="11.3671875" customWidth="true" bestFit="true"/>
+    <col min="1" max="1" width="16.41796875" customWidth="true" bestFit="true"/>
+    <col min="2" max="2" width="16.41796875" customWidth="true" bestFit="true"/>
+    <col min="3" max="3" width="9.79296875" customWidth="true" bestFit="true" hidden="true"/>
+    <col min="4" max="4" width="7.046875" customWidth="true" bestFit="true" hidden="true"/>
+    <col min="5" max="5" width="5.30078125" customWidth="true" bestFit="true"/>
+    <col min="6" max="6" width="3.953125" customWidth="true" bestFit="true"/>
+    <col min="7" max="7" width="4.265625" customWidth="true" bestFit="true"/>
+    <col min="8" max="8" width="12.6875" customWidth="true" bestFit="true"/>
+    <col min="9" max="9" width="10.51171875" customWidth="true" bestFit="true"/>
     <col min="10" max="10" width="20.703125" customWidth="true" bestFit="true"/>
-    <col min="11" max="11" width="8.609375" customWidth="true" bestFit="true"/>
+    <col min="11" max="11" width="8.3984375" customWidth="true" bestFit="true"/>
     <col min="12" max="12" width="100.703125" customWidth="true" bestFit="true"/>
     <col min="13" max="13" width="100.703125" customWidth="true" bestFit="true"/>
     <col min="14" max="14" width="100.703125" customWidth="true" bestFit="true"/>
-    <col min="15" max="15" width="13.4296875" customWidth="true" bestFit="true"/>
+    <col min="15" max="15" width="12.26171875" customWidth="true" bestFit="true"/>
     <col min="16" max="16" width="20.703125" customWidth="true" bestFit="true"/>
     <col min="17" max="17" width="20.703125" customWidth="true" bestFit="true"/>
     <col min="18" max="18" width="20.703125" customWidth="true" bestFit="true"/>
     <col min="19" max="19" width="20.703125" customWidth="true" bestFit="true"/>
     <col min="20" max="20" width="8.53515625" customWidth="true" bestFit="true"/>
-    <col min="21" max="21" width="14.72265625" customWidth="true" bestFit="true"/>
-    <col min="22" max="22" width="15.13671875" customWidth="true" bestFit="true"/>
-    <col min="23" max="23" width="16.3203125" customWidth="true" bestFit="true"/>
-    <col min="24" max="24" width="16.16796875" customWidth="true" bestFit="true"/>
-    <col min="25" max="25" width="18.49609375" customWidth="true" bestFit="true"/>
-    <col min="26" max="26" width="16.828125" customWidth="true" bestFit="true"/>
-    <col min="27" max="27" width="5.44140625" customWidth="true" bestFit="true"/>
-    <col min="28" max="28" width="19.4765625" customWidth="true" bestFit="true"/>
-    <col min="29" max="29" width="36.0390625" customWidth="true" bestFit="true"/>
-    <col min="30" max="30" width="14.7578125" customWidth="true" bestFit="true"/>
-    <col min="31" max="31" width="12.359375" customWidth="true" bestFit="true" hidden="true"/>
-    <col min="32" max="32" width="15.59375" customWidth="true" bestFit="true" hidden="true"/>
-    <col min="33" max="33" width="9.046875" customWidth="true" bestFit="true" hidden="true"/>
-    <col min="34" max="34" width="9.46484375" customWidth="true" bestFit="true"/>
+    <col min="21" max="21" width="13.609375" customWidth="true" bestFit="true"/>
+    <col min="22" max="22" width="13.91796875" customWidth="true" bestFit="true"/>
+    <col min="23" max="23" width="15.01171875" customWidth="true" bestFit="true"/>
+    <col min="24" max="24" width="14.62890625" customWidth="true" bestFit="true"/>
+    <col min="25" max="25" width="17.08203125" customWidth="true" bestFit="true"/>
+    <col min="26" max="26" width="15.18359375" customWidth="true" bestFit="true"/>
+    <col min="27" max="27" width="5.07421875" customWidth="true" bestFit="true"/>
+    <col min="28" max="28" width="17.98046875" customWidth="true" bestFit="true"/>
+    <col min="29" max="29" width="34.578125" customWidth="true" bestFit="true"/>
+    <col min="30" max="30" width="13.54296875" customWidth="true" bestFit="true"/>
+    <col min="31" max="31" width="11.3203125" customWidth="true" bestFit="true" hidden="true"/>
+    <col min="32" max="32" width="15.046875" customWidth="true" bestFit="true" hidden="true"/>
+    <col min="33" max="33" width="8.22265625" customWidth="true" bestFit="true" hidden="true"/>
+    <col min="34" max="34" width="8.53125" customWidth="true" bestFit="true"/>
     <col min="35" max="35" width="100.703125" customWidth="true"/>
-    <col min="37" max="37" width="21.4140625" customWidth="true" bestFit="true"/>
+    <col min="37" max="37" width="19.5625" customWidth="true" bestFit="true"/>
   </cols>
   <sheetData>
     <row r="1">

</xml_diff>

<commit_message>
feat: bump to 0.9.24 (#11)
</commit_message>
<xml_diff>
--- a/site/StructureDefinition-appointment-mode.xlsx
+++ b/site/StructureDefinition-appointment-mode.xlsx
@@ -30,7 +30,7 @@
     <t>Version</t>
   </si>
   <si>
-    <t>0.9.23</t>
+    <t>0.9.24</t>
   </si>
   <si>
     <t>Name</t>
@@ -57,7 +57,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2025-12-02T11:10:54-03:00</t>
+    <t>2025-12-08T15:17:38-05:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -663,42 +663,42 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" width="16.80078125" customWidth="true" bestFit="true"/>
-    <col min="2" max="2" width="16.80078125" customWidth="true" bestFit="true"/>
-    <col min="3" max="3" width="10.8515625" customWidth="true" bestFit="true" hidden="true"/>
-    <col min="4" max="4" width="7.6796875" customWidth="true" bestFit="true" hidden="true"/>
-    <col min="5" max="5" width="5.80859375" customWidth="true" bestFit="true"/>
-    <col min="6" max="6" width="4.23828125" customWidth="true" bestFit="true"/>
-    <col min="7" max="7" width="4.65625" customWidth="true" bestFit="true"/>
-    <col min="8" max="8" width="13.953125" customWidth="true" bestFit="true"/>
-    <col min="9" max="9" width="11.3671875" customWidth="true" bestFit="true"/>
+    <col min="1" max="1" width="16.41796875" customWidth="true" bestFit="true"/>
+    <col min="2" max="2" width="16.41796875" customWidth="true" bestFit="true"/>
+    <col min="3" max="3" width="9.79296875" customWidth="true" bestFit="true" hidden="true"/>
+    <col min="4" max="4" width="7.046875" customWidth="true" bestFit="true" hidden="true"/>
+    <col min="5" max="5" width="5.30078125" customWidth="true" bestFit="true"/>
+    <col min="6" max="6" width="3.953125" customWidth="true" bestFit="true"/>
+    <col min="7" max="7" width="4.265625" customWidth="true" bestFit="true"/>
+    <col min="8" max="8" width="12.6875" customWidth="true" bestFit="true"/>
+    <col min="9" max="9" width="10.51171875" customWidth="true" bestFit="true"/>
     <col min="10" max="10" width="20.703125" customWidth="true" bestFit="true"/>
-    <col min="11" max="11" width="8.609375" customWidth="true" bestFit="true"/>
+    <col min="11" max="11" width="8.3984375" customWidth="true" bestFit="true"/>
     <col min="12" max="12" width="100.703125" customWidth="true" bestFit="true"/>
     <col min="13" max="13" width="100.703125" customWidth="true" bestFit="true"/>
     <col min="14" max="14" width="100.703125" customWidth="true" bestFit="true"/>
-    <col min="15" max="15" width="13.4296875" customWidth="true" bestFit="true"/>
+    <col min="15" max="15" width="12.26171875" customWidth="true" bestFit="true"/>
     <col min="16" max="16" width="20.703125" customWidth="true" bestFit="true"/>
     <col min="17" max="17" width="20.703125" customWidth="true" bestFit="true"/>
     <col min="18" max="18" width="20.703125" customWidth="true" bestFit="true"/>
     <col min="19" max="19" width="20.703125" customWidth="true" bestFit="true"/>
     <col min="20" max="20" width="8.53515625" customWidth="true" bestFit="true"/>
-    <col min="21" max="21" width="14.72265625" customWidth="true" bestFit="true"/>
-    <col min="22" max="22" width="15.13671875" customWidth="true" bestFit="true"/>
-    <col min="23" max="23" width="16.3203125" customWidth="true" bestFit="true"/>
-    <col min="24" max="24" width="16.16796875" customWidth="true" bestFit="true"/>
-    <col min="25" max="25" width="18.49609375" customWidth="true" bestFit="true"/>
-    <col min="26" max="26" width="16.828125" customWidth="true" bestFit="true"/>
-    <col min="27" max="27" width="5.44140625" customWidth="true" bestFit="true"/>
-    <col min="28" max="28" width="19.4765625" customWidth="true" bestFit="true"/>
-    <col min="29" max="29" width="36.0390625" customWidth="true" bestFit="true"/>
-    <col min="30" max="30" width="14.7578125" customWidth="true" bestFit="true"/>
-    <col min="31" max="31" width="12.359375" customWidth="true" bestFit="true" hidden="true"/>
-    <col min="32" max="32" width="15.59375" customWidth="true" bestFit="true" hidden="true"/>
-    <col min="33" max="33" width="9.046875" customWidth="true" bestFit="true" hidden="true"/>
-    <col min="34" max="34" width="9.46484375" customWidth="true" bestFit="true"/>
+    <col min="21" max="21" width="13.609375" customWidth="true" bestFit="true"/>
+    <col min="22" max="22" width="13.91796875" customWidth="true" bestFit="true"/>
+    <col min="23" max="23" width="15.01171875" customWidth="true" bestFit="true"/>
+    <col min="24" max="24" width="14.62890625" customWidth="true" bestFit="true"/>
+    <col min="25" max="25" width="17.08203125" customWidth="true" bestFit="true"/>
+    <col min="26" max="26" width="15.18359375" customWidth="true" bestFit="true"/>
+    <col min="27" max="27" width="5.07421875" customWidth="true" bestFit="true"/>
+    <col min="28" max="28" width="17.98046875" customWidth="true" bestFit="true"/>
+    <col min="29" max="29" width="34.578125" customWidth="true" bestFit="true"/>
+    <col min="30" max="30" width="13.54296875" customWidth="true" bestFit="true"/>
+    <col min="31" max="31" width="11.3203125" customWidth="true" bestFit="true" hidden="true"/>
+    <col min="32" max="32" width="15.046875" customWidth="true" bestFit="true" hidden="true"/>
+    <col min="33" max="33" width="8.22265625" customWidth="true" bestFit="true" hidden="true"/>
+    <col min="34" max="34" width="8.53125" customWidth="true" bestFit="true"/>
     <col min="35" max="35" width="100.703125" customWidth="true"/>
-    <col min="37" max="37" width="21.4140625" customWidth="true" bestFit="true"/>
+    <col min="37" max="37" width="19.5625" customWidth="true" bestFit="true"/>
   </cols>
   <sheetData>
     <row r="1">

</xml_diff>

<commit_message>
feat: bump to 0.9.25
</commit_message>
<xml_diff>
--- a/site/StructureDefinition-appointment-mode.xlsx
+++ b/site/StructureDefinition-appointment-mode.xlsx
@@ -30,7 +30,7 @@
     <t>Version</t>
   </si>
   <si>
-    <t>0.9.24</t>
+    <t>0.9.25</t>
   </si>
   <si>
     <t>Name</t>
@@ -57,7 +57,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2025-12-08T15:17:38-05:00</t>
+    <t>2025-12-10T09:54:50-05:00</t>
   </si>
   <si>
     <t>Publisher</t>

</xml_diff>

<commit_message>
feat: bump to 0.9.25 (#12)
</commit_message>
<xml_diff>
--- a/site/StructureDefinition-appointment-mode.xlsx
+++ b/site/StructureDefinition-appointment-mode.xlsx
@@ -30,7 +30,7 @@
     <t>Version</t>
   </si>
   <si>
-    <t>0.9.24</t>
+    <t>0.9.25</t>
   </si>
   <si>
     <t>Name</t>
@@ -57,7 +57,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2025-12-08T15:17:38-05:00</t>
+    <t>2025-12-10T09:54:50-05:00</t>
   </si>
   <si>
     <t>Publisher</t>

</xml_diff>